<commit_message>
fix issues to get 'Cotação base' and 'Data de pagamento'
</commit_message>
<xml_diff>
--- a/stock_info.xlsx
+++ b/stock_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,16 @@
           <t>Próximo Rendimento %</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Próxima Cotação base</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Próxima data de pagamento</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -518,22 +528,32 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>67,59</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0,4600</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>0,6133</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>75,00</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>0,4600</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0,6133</t>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>15/06/2023</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add formatted cell to P/VP
</commit_message>
<xml_diff>
--- a/stock_info.xlsx
+++ b/stock_info.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -29,12 +29,24 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +67,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,60 +512,122 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>HGLG11</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>158,05</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>1,04</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>10,44</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1,1000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0,6770</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>162,49</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>15/05/2023</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1,1000</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0,6919</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>158,98</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>15/06/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>JSRE11</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>74,03</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>0,66</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>7,78</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>0,4600</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>0,6806</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>67,59</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>15/05/2023</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>0,4600</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>0,6133</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>75,00</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>15/06/2023</t>
         </is>

</xml_diff>

<commit_message>
add a simple interface
</commit_message>
<xml_diff>
--- a/stock_info.xlsx
+++ b/stock_info.xlsx
@@ -29,18 +29,12 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
-        <bgColor rgb="00FFFF00"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -67,13 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -512,37 +505,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HGLG11</t>
+          <t>HGBS11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>158,05</t>
+          <t>205,92</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>1,04</t>
+          <t>0,94</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10,44</t>
+          <t>8,08</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1,1000</t>
+          <t>1,4500</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0,6770</t>
+          <t>0,7287</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>162,49</t>
+          <t>198,98</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -552,17 +545,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1,1000</t>
+          <t>1,4500</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0,6919</t>
+          <t>0,6961</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>158,98</t>
+          <t>208,31</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -574,62 +567,62 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>JSRE11</t>
+          <t>LVBI11</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>74,03</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>0,66</t>
+          <t>111,63</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>0,96</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>7,78</t>
+          <t>8,05</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0,4600</t>
+          <t>0,7600</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0,6806</t>
+          <t>0,7423</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>67,59</t>
+          <t>102,39</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>15/05/2023</t>
+          <t>08/05/2023</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0,4600</t>
+          <t>0,7600</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0,6133</t>
+          <t>0,7206</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>75,00</t>
+          <t>105,47</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>15/06/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
     </row>

</xml_diff>